<commit_message>
Updated Nodes sheet in raw.xlsx
</commit_message>
<xml_diff>
--- a/raw/out.xlsx
+++ b/raw/out.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianesamson/Projects/cnet-analysis/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7291B4-8196-6F45-86E4-B1EE585EE0EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9D2B39-781D-8D43-BE35-4CB13F85CBFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
     <sheet name="Nodes" sheetId="3" r:id="rId2"/>
-    <sheet name="MERGED_TO" sheetId="4" r:id="rId3"/>
-    <sheet name="SPLIT_INTO" sheetId="5" r:id="rId4"/>
-    <sheet name="ACTIVE_IN" sheetId="2" r:id="rId5"/>
+    <sheet name="MERGED_TO" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="SPLIT_INTO" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="ACTIVE_IN" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -11575,7 +11575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14473BC5-CA06-354C-93C5-FC7E59939184}">
   <dimension ref="A1:N440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Split opponent countries and groups
</commit_message>
<xml_diff>
--- a/raw/out.xlsx
+++ b/raw/out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianesamson/Projects/cnet-analysis/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4906D229-44B5-AC40-9C7B-E70F3FC5B62A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703CF236-4683-A44F-9920-77EC41772628}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-17700" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3186" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3241" uniqueCount="1830">
   <si>
     <t>Active</t>
   </si>
@@ -4812,30 +4812,6 @@
     <t>Political Wing;Sanjukta Mukti Fouj</t>
   </si>
   <si>
-    <t>opponent</t>
-  </si>
-  <si>
-    <t>Philippines;Australia;Canada;Indonesia;Japan;Malaysia;United Kingdom;United States of America;Vietnam;Moro National Liberation Front;Moro Islamic Liberation Front</t>
-  </si>
-  <si>
-    <t>Transitional Federal Government;Ethiopia;United States of America;Somali Salvation Democratic Front;Isaaq clan;Dhulbahante clan;Absguul clan</t>
-  </si>
-  <si>
-    <t>Syria;Lebanon;Iran;Russia;Iraq;United States of America;Syrian Democratic Forces;People's Protection Units;Army of Revolutionaries;Free Syrian Army;Ahrar al-Sham;Suqour al-Sham Brigade;Hezbollah;Kata'ib Hezbollah;Asa'ib Ahl al-Haq;Al-Abbas brigade;Kata'ib Sayyid al-Shuhada;Harakat Hezbollah al-Nujaba;Houthis;Islamic State and Islamic State affiliates;Islamic State of Iraq and the Levant;Yarmouk Martyrs Brigade;Jaysh al-Jihad;Islamic Muthanna Movement</t>
-  </si>
-  <si>
-    <t>NATO;ISAF;United States of America;United Kingdom;France;Russia;China;Islamic State of Iraq and the Levant;Hezbollah;Hamas;Houthis;Southern Movement</t>
-  </si>
-  <si>
-    <t>Yemen;Saudi Arabia;United Arab Emirates;United Kingdom;United States of America;NATO;Houthis;Southern Movement;Islamic State of Iraq and the Levant - Yemen Province</t>
-  </si>
-  <si>
-    <t>India;Bangladesh;Myanmar;United States;UNLFW;CorCom</t>
-  </si>
-  <si>
-    <t>Algeria;Niger;Mauritania;Mali;Tunisia;Libya;France;Morocco;Chad;Nigeria;United States of America;Islamic State of Iraq and the Levant - Libyan Province</t>
-  </si>
-  <si>
     <t>Tripura</t>
   </si>
   <si>
@@ -4845,84 +4821,18 @@
     <t>Tunisia;Algeria;Libya</t>
   </si>
   <si>
-    <t>Peshmerga;Iraq;Syria;Syrian Democratic Forces;United States of America</t>
-  </si>
-  <si>
-    <t>Mahdi Army;Iraq</t>
-  </si>
-  <si>
     <t>Egypt;Israel;Palestine</t>
   </si>
   <si>
-    <t>Mali;Senegal;Mauritania;United States of America;France;National Movement for the Liberation of Azawad</t>
-  </si>
-  <si>
     <t>Nigeria;Mali</t>
   </si>
   <si>
-    <t>Iraq;Popular Mobilization Forces;Asa'ib Ahl al-Haq;Kata'ib Hezbollah;Badr Brigades;Promised Day Brigades;Kurdistan Regional Government;Peshmerga;Iran;Islamic State of Iraq and Levant</t>
-  </si>
-  <si>
-    <t>Iraq;United States of America;United Kingdom;Islamic State of Iraq and the Levant;Al-Qaida in Iraq;Army of the Men of the Naqshbandi Order;Free Syrian Army;Islamic Front;Al-Nusra Front;Kurdistan Workers' Party;White Flags;Army of Conquest;Peshmerga</t>
-  </si>
-  <si>
     <t>Nigeria;Cameroon;Niger;Chad;Benin</t>
   </si>
   <si>
-    <t>Russia;Chechnya;Dagestan;Ingushetia;Kabardino-Balkaria;Karachay-Cherkessia;North Ossetia-Alania;Adygea;Krasnodar Krai;Stavropol Krai;Azerbaijan;Georgia;Armenia;Syria;Rojava;Iraq;Iran;Pakistan;India;NATO</t>
-  </si>
-  <si>
     <t>British Government;British Army;Police Service of Northern Ireland;An Garda Siochana;Irish Army</t>
   </si>
   <si>
-    <t>China;Pakistan;India;Jordan;Kazakhstan;Kyrgyzstan;Mongolia;Russia;Tajikistan;Turkmenistan;United Arab Emirates;Uzbekistan;United States of America;Syria;Syrian Armed Forces;National Defence Force;Liwa Fatemiyoun;Cyprus;Iraqi Shia militiasPeople's Protection Units;Syrian Democratic Forces;Hezbollah;Iranian Revolutionary Guard Corps</t>
-  </si>
-  <si>
-    <t>Islamic Republic of Afghanistan;NATO;Resolute Support Mission</t>
-  </si>
-  <si>
-    <t>Iraq;Islamic State of Iraq and the Levant;Free Syrian Army;Islamic Front;Ahrar al-Sham;Al-Nusra Front;Ajnad al-Sham;Tahrir al-Sham;Peshmerga;Army of Conquest</t>
-  </si>
-  <si>
-    <t>Syria;National Defense Force;Syrian Democratic Forces;Hezbollah;Liwa Fatemiyoun;Iran</t>
-  </si>
-  <si>
-    <t>Turkey;PKK</t>
-  </si>
-  <si>
-    <t>Yemen;Saudi Arabia;United Arab Emirates;Morocco;Senegal;Sudan;Somalia;United States of America;Israe;Bahrain;Egypt;AQAP;Islamic State of Iraq and the Levant - Yemen Province;Academi</t>
-  </si>
-  <si>
-    <t>United Kingdom;Republic of Ireland;Irish People's Liberation Organisation</t>
-  </si>
-  <si>
-    <t>United Kingdom;Royal Ulster Constabulary;British Army;Ulster Defence Association;Red Hand Commando;Ulster Volunteer Force;Irish National Liberation Army;Provisional IRA;IPLO Belfast Brigade</t>
-  </si>
-  <si>
-    <t>Afghanistan;Uzbekistan;China;ISAF;Germany;United States of America;Russia;Pakistan;India;Qatar</t>
-  </si>
-  <si>
-    <t>Uzbekistan;China;Russia;Kazakhstan;Kyrgyzstan;Tajikistan;Turkmenistan;United States of America;Pakistan;India;Afghanistan;International Security Assistance Force</t>
-  </si>
-  <si>
-    <t>Afghanistan;Algeria;Australia;Belgium;Canada;China;Denmark;Egypt;Estonia;Fiji;France;Greece;India;Indonesia;Iran;Iraq;Iraqi Kurdistan;Israel;Italy;Latvia;Lebanon;Libya;Lithuania;Netherlands;Pakistan;Philippines;Russia;Saudi Arabia;Syria;Tajikistan;Tunisia;Turkey;United Kingdom;United States of America;Syrian Democratic Forces;Nineveh Plain Protection Units;Hezbollah;Badr Organisation;Asa'ib Ahl al-Haq;Kata'ib Hezbollah;Harakat Hezbollah al-Nujaba;Kata'ib Sayyid al-Shuhada;Peshmerga;Kurdistan Communities Union;Free Syrian Army;al-Qaeda;Ahrar al-Sham;Al-Nusra Front;Libya Shield Force;Hamas;Shura Council of Mujahideen in Derna;Taliban;Army of Conquest</t>
-  </si>
-  <si>
-    <t>Russia;Georgia;Azerbaijan;Armenia;South Ossetia;Abkhazia;Artsakh</t>
-  </si>
-  <si>
-    <t>Afghanistan;Pakistan;United States of America;Taliban;Tehrik-i-Taliban</t>
-  </si>
-  <si>
-    <t>Libya;New General National Congress;Libya Shield Force;Shura Council of Mujahideen in Derna;Abu Salim Martyrs Brigade;Egypt;United States of America</t>
-  </si>
-  <si>
-    <t>Yemen;Saudi Arabia;Houthis;Al-Qaeda in the Arabian Peninsula;Southern Movement</t>
-  </si>
-  <si>
-    <t>Afghanistan;NATO;ISAF</t>
-  </si>
-  <si>
     <t>Mali;Algeria;Tunisia;Niger;Libya;France;United States of America</t>
   </si>
   <si>
@@ -4932,66 +4842,27 @@
     <t>United Nations;United States of America;United Kingdom;France;Russia;China;Netherlands;Sweden;Poland;Brunei;Indonesia;Malaysia;Myanmar;Philippines;Singapore;Thailand;Vietnam;Kazakhstan;Pakistan;Uzbekistan</t>
   </si>
   <si>
-    <t>Syria;Iran;Russia;United States of America;Ahrar al-Sham;Suqour al-Sham Brigade;Sham Legion;Free Syrian Army;Tahrir al-Sham</t>
-  </si>
-  <si>
-    <t>Algeria;Morocco;Tunisia;Western Sahara</t>
-  </si>
-  <si>
-    <t>Syrian Armed Forces;Islamic State of Iraq and the Levant;Syrian Democratic Forces;Afghan National Security Forces</t>
-  </si>
-  <si>
-    <t>Iraq;United States of America;Israel;Islamic State of Iraq and the Levant;Mojahedin-e Khalq;Free Syrian Army;Peshmerga</t>
-  </si>
-  <si>
-    <t>Irish republicans;Irish nationalists;Irish Catholics;British Army;Royal Ulster Constabulary;Police Service of Northern Ireland;Ulster Volunteer Force</t>
-  </si>
-  <si>
     <t>Morocco;Iraq</t>
   </si>
   <si>
     <t>Indonesia;Turkey;United States of America</t>
   </si>
   <si>
-    <t>Israel;Egypt;Hamas</t>
-  </si>
-  <si>
     <t>India;Bhutan</t>
   </si>
   <si>
     <t>India;Myanmar</t>
   </si>
   <si>
-    <t>United States of America;Iraq;MNF-I;Free Syrian Army;Islamic State of Iraq and the Levant</t>
-  </si>
-  <si>
-    <t>United Kingdom;British Army;Royal Ulster Constabulary;Ulster loyalist paramilitaries;Official IRA;Irish People's Liberation Organisation</t>
-  </si>
-  <si>
-    <t>British Army;Police Service of Northern Ireland;An Garda Siochana;Irish Defence Forces</t>
-  </si>
-  <si>
     <t>Colombia;United States of America</t>
   </si>
   <si>
-    <t>Syria;Iran;Russia;Lebanon;United States;Turkey;Syrian Democratic Forces;Liwa Zainebiyoun;Liwa Fatemiyoun;Free Syrian Army;Syrian National Army;National Front for Liberation;National Liberation Movement;Men of God Brigade;Hezbollah;Al-Abbas brigade;Harakat Hezbollah al-Nujaba;Islamic State</t>
-  </si>
-  <si>
-    <t>Afghanistan;India;United States of America;NATO;ISAF;Islamic State of Iraq and the Levant - Khorasan Province;Khorasan Province;Jamiat-e Islami;Junbish-i-Milli;Hezbe Wahdat</t>
-  </si>
-  <si>
     <t>United States of America;Pakistan</t>
   </si>
   <si>
     <t>Irish Republican Army;Irish National Liberation Army;Irish People's Liberation Organization;Irish republicans;Irish nationalists</t>
   </si>
   <si>
-    <t>Provisional IRA;Official IRA;Irish National Liberation Army;Irish People's Liberation Organization;Irish republicans;Irish nationalists;An Garda Siochana;British Army;Loyalist Volunteer Force</t>
-  </si>
-  <si>
-    <t>Syria;al-Nusra Front;Free Syrian Army</t>
-  </si>
-  <si>
     <t>battles</t>
   </si>
   <si>
@@ -5425,6 +5296,234 @@
   </si>
   <si>
     <t>Australia;Canada;Japan;New Zealand;United Kingdom;United States of America</t>
+  </si>
+  <si>
+    <t>opponent_country</t>
+  </si>
+  <si>
+    <t>opponent_group</t>
+  </si>
+  <si>
+    <t>opponent_entity</t>
+  </si>
+  <si>
+    <t>Philippines;Australia;Canada;Indonesia;Japan;Malaysia;United Kingdom;United States of America;Vietnam</t>
+  </si>
+  <si>
+    <t>Moro National Liberation Front;Moro Islamic Liberation Front</t>
+  </si>
+  <si>
+    <t>Transitional Federal Government</t>
+  </si>
+  <si>
+    <t>Ethiopia;United States of America</t>
+  </si>
+  <si>
+    <t>Somali Salvation Democratic Front;Isaaq clan;Dhulbahante clan;Absguul clan</t>
+  </si>
+  <si>
+    <t>People's Protection Units;Army of Revolutionaries;Free Syrian Army;Ahrar al-Sham;Suqour al-Sham Brigade;Hezbollah;Kata'ib Hezbollah;Asa'ib Ahl al-Haq;Al-Abbas brigade;Kata'ib Sayyid al-Shuhada;Harakat Hezbollah al-Nujaba;Houthis;Islamic State and Islamic State affiliates;Islamic State of Iraq and the Levant;Yarmouk Martyrs Brigade;Jaysh al-Jihad;Islamic Muthanna Movement</t>
+  </si>
+  <si>
+    <t>Syria;Lebanon;Iran;Russia;Iraq;United States of America</t>
+  </si>
+  <si>
+    <t>Syrian Democratic Forces</t>
+  </si>
+  <si>
+    <t>NATO;ISAF</t>
+  </si>
+  <si>
+    <t>United States of America;United Kingdom;France;Russia;China</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant;Hezbollah;Hamas;Houthis;Southern Movement</t>
+  </si>
+  <si>
+    <t>Houthis;Southern Movement;Islamic State of Iraq and the Levant - Yemen Province</t>
+  </si>
+  <si>
+    <t>Yemen;Saudi Arabia;United Arab Emirates;United Kingdom;United States of America</t>
+  </si>
+  <si>
+    <t>NATO</t>
+  </si>
+  <si>
+    <t>UNLFW;CorCom</t>
+  </si>
+  <si>
+    <t>India;Bangladesh;Myanmar;United States of America</t>
+  </si>
+  <si>
+    <t>Algeria;Niger;Mauritania;Mali;Tunisia;Libya;France;Morocco;Chad;Nigeria;United States of America</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant - Libyan Province</t>
+  </si>
+  <si>
+    <t>Iraq;Syria;United States of America</t>
+  </si>
+  <si>
+    <t>Peshmerga;Syrian Democratic Forces</t>
+  </si>
+  <si>
+    <t>Mali;Senegal;Mauritania;United States of America;France</t>
+  </si>
+  <si>
+    <t>National Movement for the Liberation of Azawad</t>
+  </si>
+  <si>
+    <t>Popular Mobilization Forces;Asa'ib Ahl al-Haq;Kata'ib Hezbollah;Badr Brigades;Promised Day Brigades;Kurdistan Regional Government;Peshmerga;Iran;Islamic State of Iraq and Levant</t>
+  </si>
+  <si>
+    <t>Iraq;United States of America;United Kingdom</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant;Al-Qaida in Iraq;Army of the Men of the Naqshbandi Order;Free Syrian Army;Islamic Front;Al-Nusra Front;Kurdistan Workers' Party;White Flags;Army of Conquest;Peshmerga</t>
+  </si>
+  <si>
+    <t>Russia;Azerbaijan;Georgia;Armenia;Syria;Iraq;Iran;Pakistan;India</t>
+  </si>
+  <si>
+    <t>NATO;Rojava;Chechnya;Dagestan;Ingushetia;Kabardino-Balkaria;Karachay-Cherkessia;North Ossetia-Alania;Adygea;Krasnodar Krai;Stavropol Krai</t>
+  </si>
+  <si>
+    <t>China;Pakistan;India;Jordan;Kazakhstan;Kyrgyzstan;Mongolia;Russia;Tajikistan;Turkmenistan;United Arab Emirates;Uzbekistan;United States of America;Syria</t>
+  </si>
+  <si>
+    <t>Resolute Support Mission</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant;Free Syrian Army;Islamic Front;Ahrar al-Sham;Al-Nusra Front;Ajnad al-Sham;Tahrir al-Sham;Peshmerga;Army of Conquest</t>
+  </si>
+  <si>
+    <t>Hezbollah;Liwa Fatemiyoun;</t>
+  </si>
+  <si>
+    <t>National Defense Force;Syrian Democratic Forces</t>
+  </si>
+  <si>
+    <t>Liwa Fatemiyoun;Cyprus;Iraqi Shia militiasPeople's Protection Units;Syrian Democratic Forces;Hezbollah;Iranian Revolutionary Guard Corps</t>
+  </si>
+  <si>
+    <t>Syrian Armed Forces;National Defence Force</t>
+  </si>
+  <si>
+    <t>PKK</t>
+  </si>
+  <si>
+    <t>AQAP;Islamic State of Iraq and the Levant - Yemen Province;Academi</t>
+  </si>
+  <si>
+    <t>Yemen;Saudi Arabia;United Arab Emirates;Morocco;Senegal;Sudan;Somalia;United States of America;Israel;Bahrain;Egypt</t>
+  </si>
+  <si>
+    <t>United Kingdom;Ireland</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Royal Ulster Constabulary;British Army;Ulster Defence Association;Red Hand Commando;Ulster Volunteer Force;Irish National Liberation Army;Provisional IRA;IPLO Belfast Brigade</t>
+  </si>
+  <si>
+    <t>Afghanistan;Uzbekistan;China;Germany;United States of America;Russia;Pakistan;India;Qatar</t>
+  </si>
+  <si>
+    <t>ISAF</t>
+  </si>
+  <si>
+    <t>Uzbekistan;China;Russia;Kazakhstan;Kyrgyzstan;Tajikistan;Turkmenistan;United States of America;Pakistan;India;Afghanistan</t>
+  </si>
+  <si>
+    <t>Nineveh Plain Protection Units;Hezbollah;Badr Organisation;Asa'ib Ahl al-Haq;Kata'ib Hezbollah;Harakat Hezbollah al-Nujaba;Kata'ib Sayyid al-Shuhada;Peshmerga;Kurdistan Communities Union;Free Syrian Army;al-Qaeda;Ahrar al-Sham;Al-Nusra Front;Libya Shield Force;Hamas;Shura Council of Mujahideen in Derna;Taliban;Army of Conquest</t>
+  </si>
+  <si>
+    <t>Afghanistan;Algeria;Australia;Belgium;Canada;China;Denmark;Egypt;Estonia;Fiji;France;Greece;India;Indonesia;Iran;Iraq;Iraqi Kurdistan;Israel;Italy;Latvia;Lebanon;Libya;Lithuania;Netherlands;Pakistan;Philippines;Russia;Saudi Arabia;Syria;Tajikistan;Tunisia;Turkey;United Kingdom;United States of America</t>
+  </si>
+  <si>
+    <t>Russia;Georgia;Azerbaijan;Armenia</t>
+  </si>
+  <si>
+    <t>South Ossetia;Abkhazia;Artsakh</t>
+  </si>
+  <si>
+    <t>Afghanistan;Pakistan;United States of America</t>
+  </si>
+  <si>
+    <t>Taliban;Tehrik-i-Taliban</t>
+  </si>
+  <si>
+    <t>Libya;Egypt;United States of America</t>
+  </si>
+  <si>
+    <t>New General National Congress;Libya Shield Force;Shura Council of Mujahideen in Derna;Abu Salim Martyrs Brigade</t>
+  </si>
+  <si>
+    <t>Houthis;Al-Qaeda in the Arabian Peninsula;Southern Movement</t>
+  </si>
+  <si>
+    <t>Syria;Iran;Russia;United States of America</t>
+  </si>
+  <si>
+    <t>Ahrar al-Sham;Suqour al-Sham Brigade;Sham Legion;Free Syrian Army;Tahrir al-Sham</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Algeria;Morocco;Tunisia</t>
+  </si>
+  <si>
+    <t>Syrian Armed Forces;Syrian Democratic Forces;Afghan National Security Forces</t>
+  </si>
+  <si>
+    <t>Iraq;United States of America;Israel</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant;Mojahedin-e Khalq;Free Syrian Army;Peshmerga</t>
+  </si>
+  <si>
+    <t>Irish republicans;Irish nationalists;Irish Catholics;Royal Ulster Constabulary;Police Service of Northern Ireland;Ulster Volunteer Force</t>
+  </si>
+  <si>
+    <t>British Army</t>
+  </si>
+  <si>
+    <t>Israel;Egypt</t>
+  </si>
+  <si>
+    <t>United States of America;Iraq</t>
+  </si>
+  <si>
+    <t>MNF-I;Free Syrian Army;Islamic State of Iraq and the Levant</t>
+  </si>
+  <si>
+    <t>Royal Ulster Constabulary;Ulster loyalist paramilitaries;Official IRA;Irish People's Liberation Organisation</t>
+  </si>
+  <si>
+    <t>British Army;Police Service of Northern Ireland;Irish Defence Forces</t>
+  </si>
+  <si>
+    <t>An Garda Siochana</t>
+  </si>
+  <si>
+    <t>Liwa Zainebiyoun;Liwa Fatemiyoun;Free Syrian Army;Syrian National Army;National Front for Liberation;National Liberation Movement;Men of God Brigade;Hezbollah;Al-Abbas brigade;Harakat Hezbollah al-Nujaba;Islamic State</t>
+  </si>
+  <si>
+    <t>Syria;Iran;Russia;Lebanon;United States;Turkey</t>
+  </si>
+  <si>
+    <t>Afghanistan;India;United States of America</t>
+  </si>
+  <si>
+    <t>Islamic State of Iraq and the Levant - Khorasan Province;Khorasan Province;Jamiat-e Islami;Junbish-i-Milli;Hezbe Wahdat</t>
+  </si>
+  <si>
+    <t>Provisional IRA;Official IRA;Irish National Liberation Army;Irish People's Liberation Organization;Irish republicans;Irish nationalists;An Garda Siochana;Loyalist Volunteer Force</t>
+  </si>
+  <si>
+    <t>al-Nusra Front;Free Syrian Army</t>
   </si>
 </sst>
 </file>
@@ -11646,10 +11745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14473BC5-CA06-354C-93C5-FC7E59939184}">
-  <dimension ref="A1:R440"/>
+  <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11664,12 +11763,12 @@
     <col min="12" max="13" width="47.83203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="49.6640625" style="15" customWidth="1"/>
     <col min="15" max="15" width="27" style="15" customWidth="1"/>
-    <col min="16" max="16" width="29.1640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="51.83203125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="51.1640625" style="15" customWidth="1"/>
+    <col min="16" max="18" width="29.1640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="51.83203125" style="13" customWidth="1"/>
+    <col min="20" max="20" width="51.1640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>1356</v>
       </c>
@@ -11686,31 +11785,31 @@
         <v>1412</v>
       </c>
       <c r="F1" t="s">
-        <v>1690</v>
+        <v>1647</v>
       </c>
       <c r="G1" t="s">
-        <v>1689</v>
+        <v>1646</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>1431</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>1759</v>
+        <v>1716</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>1758</v>
+        <v>1715</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>1762</v>
+        <v>1719</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1761</v>
+        <v>1718</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>1784</v>
+        <v>1741</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>1783</v>
+        <v>1740</v>
       </c>
       <c r="O1" s="15" t="s">
         <v>1490</v>
@@ -11718,14 +11817,20 @@
       <c r="P1" s="2" t="s">
         <v>1501</v>
       </c>
-      <c r="Q1" s="13" t="s">
-        <v>1592</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>1755</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>1754</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>147</v>
       </c>
@@ -11738,7 +11843,7 @@
         <v>1413</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1691</v>
+        <v>1648</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>352</v>
@@ -11755,7 +11860,7 @@
         <v>1485</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>1785</v>
+        <v>1742</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>1413</v>
@@ -11763,9 +11868,9 @@
       <c r="P2" s="2" t="s">
         <v>1502</v>
       </c>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T2" s="13"/>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>152</v>
       </c>
@@ -11794,9 +11899,9 @@
       <c r="P3" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T3" s="13"/>
+    </row>
+    <row r="4" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>153</v>
       </c>
@@ -11828,12 +11933,15 @@
       <c r="P4" s="2" t="s">
         <v>1503</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>1593</v>
-      </c>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="s">
+        <v>1758</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>1757</v>
+      </c>
+      <c r="T4" s="13"/>
+    </row>
+    <row r="5" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>162</v>
       </c>
@@ -11863,14 +11971,14 @@
       <c r="P5" s="2" t="s">
         <v>1504</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="S5" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>171</v>
       </c>
@@ -11898,12 +12006,12 @@
       <c r="P6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="S6" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T6" s="13"/>
+    </row>
+    <row r="7" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>176</v>
       </c>
@@ -11916,7 +12024,7 @@
         <v>1413</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1703</v>
+        <v>1660</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>611</v>
@@ -11935,9 +12043,9 @@
       <c r="P7" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>181</v>
       </c>
@@ -11959,10 +12067,10 @@
         <v>1413</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>1787</v>
+        <v>1744</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>1786</v>
+        <v>1743</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>1413</v>
@@ -11970,9 +12078,9 @@
       <c r="P8" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R8" s="13"/>
-    </row>
-    <row r="9" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>188</v>
       </c>
@@ -11998,9 +12106,9 @@
       <c r="P9" s="2" t="s">
         <v>1505</v>
       </c>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>191</v>
       </c>
@@ -12028,9 +12136,9 @@
       <c r="P10" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>195</v>
       </c>
@@ -12055,7 +12163,7 @@
         <v>1371</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>1788</v>
+        <v>1745</v>
       </c>
       <c r="O11" s="13" t="s">
         <v>1413</v>
@@ -12063,9 +12171,9 @@
       <c r="P11" s="2" t="s">
         <v>1506</v>
       </c>
-      <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>201</v>
       </c>
@@ -12091,9 +12199,9 @@
       <c r="P12" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T12" s="13"/>
+    </row>
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>202</v>
       </c>
@@ -12125,9 +12233,9 @@
       <c r="P13" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R13" s="13"/>
-    </row>
-    <row r="14" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>208</v>
       </c>
@@ -12140,10 +12248,10 @@
         <v>2006</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1693</v>
+        <v>1650</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>1692</v>
+        <v>1649</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -12157,12 +12265,18 @@
       <c r="P14" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q14" s="13" t="s">
-        <v>1594</v>
-      </c>
-      <c r="R14" s="13"/>
-    </row>
-    <row r="15" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q14" s="2" t="s">
+        <v>1761</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>1759</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>1760</v>
+      </c>
+      <c r="T14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>216</v>
       </c>
@@ -12190,9 +12304,9 @@
       <c r="P15" s="2" t="s">
         <v>1507</v>
       </c>
-      <c r="R15" s="13"/>
-    </row>
-    <row r="16" spans="1:18" ht="204" x14ac:dyDescent="0.2">
+      <c r="T15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" ht="221" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>222</v>
       </c>
@@ -12207,34 +12321,40 @@
         <v>2017</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>1695</v>
+        <v>1652</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>1694</v>
+        <v>1651</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>1433</v>
       </c>
       <c r="I16" s="13"/>
       <c r="K16" s="14" t="s">
-        <v>1764</v>
+        <v>1721</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>1763</v>
+        <v>1720</v>
       </c>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="2" t="s">
         <v>1508</v>
       </c>
-      <c r="Q16" s="13" t="s">
-        <v>1595</v>
-      </c>
-      <c r="R16" s="13" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="404" x14ac:dyDescent="0.2">
+      <c r="Q16" s="2" t="s">
+        <v>1762</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="S16" s="13" t="s">
+        <v>1763</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="404" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>230</v>
       </c>
@@ -12247,18 +12367,18 @@
         <v>1413</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1691</v>
+        <v>1648</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>1696</v>
+        <v>1653</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="K17" s="14" t="s">
-        <v>1766</v>
+        <v>1723</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>1765</v>
+        <v>1722</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="13" t="s">
@@ -12267,14 +12387,20 @@
       <c r="P17" s="2" t="s">
         <v>1509</v>
       </c>
-      <c r="Q17" s="13" t="s">
-        <v>1596</v>
-      </c>
-      <c r="R17" s="13" t="s">
-        <v>1654</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="170" x14ac:dyDescent="0.2">
+      <c r="Q17" s="2" t="s">
+        <v>1767</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>1765</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>1766</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="170" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>234</v>
       </c>
@@ -12287,7 +12413,7 @@
         <v>1413</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>1697</v>
+        <v>1654</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>169</v>
@@ -12297,10 +12423,10 @@
       </c>
       <c r="I18" s="13"/>
       <c r="K18" s="14" t="s">
-        <v>1764</v>
+        <v>1721</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>1767</v>
+        <v>1724</v>
       </c>
       <c r="N18" s="13"/>
       <c r="O18" s="13" t="s">
@@ -12309,14 +12435,20 @@
       <c r="P18" s="2" t="s">
         <v>1510</v>
       </c>
-      <c r="Q18" s="13" t="s">
-        <v>1597</v>
-      </c>
-      <c r="R18" s="13" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q18" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>1770</v>
+      </c>
+      <c r="S18" s="13" t="s">
+        <v>1769</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>1432</v>
       </c>
@@ -12340,7 +12472,7 @@
         <v>550</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>1768</v>
+        <v>1725</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="13" t="s">
@@ -12349,12 +12481,15 @@
       <c r="P19" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q19" s="13" t="s">
-        <v>1598</v>
-      </c>
-      <c r="R19" s="13"/>
-    </row>
-    <row r="20" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="R19" s="2" t="s">
+        <v>1771</v>
+      </c>
+      <c r="S19" s="13" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T19" s="13"/>
+    </row>
+    <row r="20" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>877</v>
       </c>
@@ -12386,14 +12521,17 @@
       <c r="P20" s="2" t="s">
         <v>1511</v>
       </c>
-      <c r="Q20" s="13" t="s">
-        <v>1599</v>
-      </c>
-      <c r="R20" s="13" t="s">
-        <v>1656</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="2" t="s">
+        <v>1774</v>
+      </c>
+      <c r="S20" s="13" t="s">
+        <v>1773</v>
+      </c>
+      <c r="T20" s="13" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>255</v>
       </c>
@@ -12419,9 +12557,9 @@
       <c r="P21" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R21" s="13"/>
-    </row>
-    <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T21" s="13"/>
+    </row>
+    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>256</v>
       </c>
@@ -12449,9 +12587,9 @@
       <c r="P22" s="2" t="s">
         <v>1512</v>
       </c>
-      <c r="R22" s="13"/>
-    </row>
-    <row r="23" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T22" s="13"/>
+    </row>
+    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>261</v>
       </c>
@@ -12464,7 +12602,7 @@
         <v>1413</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>1600</v>
+        <v>1592</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>611</v>
@@ -12481,12 +12619,12 @@
       <c r="P23" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="Q23" s="13" t="s">
-        <v>1600</v>
-      </c>
-      <c r="R23" s="13"/>
-    </row>
-    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="R23" s="13" t="s">
+        <v>1592</v>
+      </c>
+      <c r="T23" s="13"/>
+    </row>
+    <row r="24" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>266</v>
       </c>
@@ -12501,7 +12639,7 @@
         <v>2017</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>1698</v>
+        <v>1655</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>671</v>
@@ -12520,14 +12658,14 @@
       <c r="P24" s="2" t="s">
         <v>1513</v>
       </c>
-      <c r="Q24" s="13" t="s">
-        <v>1601</v>
-      </c>
       <c r="R24" s="13" t="s">
+        <v>1593</v>
+      </c>
+      <c r="T24" s="13" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>275</v>
       </c>
@@ -12557,12 +12695,12 @@
       <c r="P25" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Q25" s="13" t="s">
-        <v>1602</v>
-      </c>
-      <c r="R25" s="13"/>
-    </row>
-    <row r="26" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="S25" s="13" t="s">
+        <v>1594</v>
+      </c>
+      <c r="T25" s="13"/>
+    </row>
+    <row r="26" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>283</v>
       </c>
@@ -12579,10 +12717,10 @@
         <v>2014</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>1700</v>
+        <v>1657</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>1699</v>
+        <v>1656</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>1435</v>
@@ -12598,14 +12736,17 @@
       <c r="P26" s="2" t="s">
         <v>1514</v>
       </c>
-      <c r="Q26" s="13" t="s">
-        <v>1603</v>
-      </c>
-      <c r="R26" s="13" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="R26" s="2" t="s">
+        <v>1776</v>
+      </c>
+      <c r="S26" s="13" t="s">
+        <v>1775</v>
+      </c>
+      <c r="T26" s="13" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>292</v>
       </c>
@@ -12635,12 +12776,15 @@
       <c r="P27" s="2" t="s">
         <v>1515</v>
       </c>
-      <c r="Q27" s="13" t="s">
-        <v>1604</v>
-      </c>
-      <c r="R27" s="13"/>
-    </row>
-    <row r="28" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q27" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="T27" s="13"/>
+    </row>
+    <row r="28" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>301</v>
       </c>
@@ -12653,7 +12797,7 @@
         <v>2014</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>1701</v>
+        <v>1658</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>560</v>
@@ -12673,14 +12817,14 @@
       <c r="P28" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="Q28" s="13" t="s">
-        <v>1605</v>
-      </c>
-      <c r="R28" s="13" t="s">
+      <c r="S28" s="13" t="s">
+        <v>1595</v>
+      </c>
+      <c r="T28" s="13" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>310</v>
       </c>
@@ -12694,7 +12838,7 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="12" t="s">
-        <v>1688</v>
+        <v>1645</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -12711,12 +12855,15 @@
       <c r="P29" s="2" t="s">
         <v>1516</v>
       </c>
-      <c r="Q29" s="13" t="s">
-        <v>1606</v>
-      </c>
-      <c r="R29" s="13"/>
-    </row>
-    <row r="30" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q29" s="2" t="s">
+        <v>1778</v>
+      </c>
+      <c r="S29" s="13" t="s">
+        <v>1777</v>
+      </c>
+      <c r="T29" s="13"/>
+    </row>
+    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>315</v>
       </c>
@@ -12745,9 +12892,9 @@
       <c r="P30" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R30" s="13"/>
-    </row>
-    <row r="31" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T30" s="13"/>
+    </row>
+    <row r="31" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>318</v>
       </c>
@@ -12763,7 +12910,7 @@
         <v>320</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>1702</v>
+        <v>1659</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>1436</v>
@@ -12779,14 +12926,14 @@
       <c r="P31" s="2" t="s">
         <v>1517</v>
       </c>
-      <c r="Q31" s="13" t="s">
-        <v>1607</v>
-      </c>
-      <c r="R31" s="13" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S31" s="13" t="s">
+        <v>1596</v>
+      </c>
+      <c r="T31" s="13" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>325</v>
       </c>
@@ -12817,9 +12964,9 @@
       <c r="P32" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="R32" s="13"/>
-    </row>
-    <row r="33" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>331</v>
       </c>
@@ -12848,9 +12995,9 @@
       <c r="P33" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R33" s="13"/>
-    </row>
-    <row r="34" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T33" s="13"/>
+    </row>
+    <row r="34" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>332</v>
       </c>
@@ -12882,14 +13029,17 @@
       <c r="P34" s="2" t="s">
         <v>1519</v>
       </c>
-      <c r="Q34" s="13" t="s">
-        <v>1608</v>
-      </c>
-      <c r="R34" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="170" x14ac:dyDescent="0.2">
+      <c r="Q34" s="2" t="s">
+        <v>1779</v>
+      </c>
+      <c r="S34" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="T34" s="13" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="170" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>341</v>
       </c>
@@ -12902,34 +13052,37 @@
         <v>1413</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>1704</v>
+        <v>1661</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>1699</v>
+        <v>1656</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>1437</v>
       </c>
       <c r="I35" s="13"/>
       <c r="K35" s="14" t="s">
-        <v>1770</v>
+        <v>1727</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>1769</v>
+        <v>1726</v>
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="2" t="s">
         <v>1520</v>
       </c>
-      <c r="Q35" s="13" t="s">
-        <v>1609</v>
-      </c>
-      <c r="R35" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q35" s="2" t="s">
+        <v>1781</v>
+      </c>
+      <c r="S35" s="13" t="s">
+        <v>1780</v>
+      </c>
+      <c r="T35" s="13" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>351</v>
       </c>
@@ -12954,7 +13107,7 @@
         <v>1485</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>1789</v>
+        <v>1746</v>
       </c>
       <c r="O36" s="13" t="s">
         <v>1413</v>
@@ -12962,9 +13115,9 @@
       <c r="P36" s="2" t="s">
         <v>1521</v>
       </c>
-      <c r="R36" s="13"/>
-    </row>
-    <row r="37" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T36" s="13"/>
+    </row>
+    <row r="37" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>1381</v>
       </c>
@@ -12994,9 +13147,9 @@
       <c r="P37" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R37" s="13"/>
-    </row>
-    <row r="38" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T37" s="13"/>
+    </row>
+    <row r="38" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>371</v>
       </c>
@@ -13024,9 +13177,9 @@
       <c r="P38" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="R38" s="13"/>
-    </row>
-    <row r="39" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T38" s="13"/>
+    </row>
+    <row r="39" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>378</v>
       </c>
@@ -13056,9 +13209,9 @@
       <c r="P39" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R39" s="13"/>
-    </row>
-    <row r="40" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T39" s="13"/>
+    </row>
+    <row r="40" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>388</v>
       </c>
@@ -13071,10 +13224,10 @@
         <v>1413</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>1706</v>
+        <v>1663</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>1705</v>
+        <v>1662</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -13091,14 +13244,14 @@
       <c r="P40" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="Q40" s="13" t="s">
+      <c r="S40" s="13" t="s">
         <v>550</v>
       </c>
-      <c r="R40" s="13" t="s">
+      <c r="T40" s="13" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>396</v>
       </c>
@@ -13111,10 +13264,10 @@
         <v>1413</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>1708</v>
+        <v>1665</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>1707</v>
+        <v>1664</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
@@ -13131,14 +13284,14 @@
       <c r="P41" s="2" t="s">
         <v>1522</v>
       </c>
-      <c r="Q41" s="13" t="s">
-        <v>1610</v>
-      </c>
-      <c r="R41" s="13" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="S41" s="13" t="s">
+        <v>1597</v>
+      </c>
+      <c r="T41" s="13" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>403</v>
       </c>
@@ -13156,7 +13309,7 @@
         <v>405</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>1709</v>
+        <v>1666</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
@@ -13173,14 +13326,17 @@
       <c r="P42" s="2" t="s">
         <v>1523</v>
       </c>
-      <c r="Q42" s="13" t="s">
-        <v>1611</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R42" s="2" t="s">
+        <v>1783</v>
+      </c>
+      <c r="S42" s="13" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T42" s="13" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>1218</v>
       </c>
@@ -13209,9 +13365,9 @@
       <c r="P43" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="R43" s="13"/>
-    </row>
-    <row r="44" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T43" s="13"/>
+    </row>
+    <row r="44" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>410</v>
       </c>
@@ -13239,9 +13395,9 @@
       <c r="P44" s="2" t="s">
         <v>1524</v>
       </c>
-      <c r="R44" s="13"/>
-    </row>
-    <row r="45" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T44" s="13"/>
+    </row>
+    <row r="45" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>1220</v>
       </c>
@@ -13269,9 +13425,9 @@
       <c r="P45" s="2" t="s">
         <v>1524</v>
       </c>
-      <c r="R45" s="13"/>
-    </row>
-    <row r="46" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T45" s="13"/>
+    </row>
+    <row r="46" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>428</v>
       </c>
@@ -13304,9 +13460,9 @@
       <c r="P46" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="R46" s="13"/>
-    </row>
-    <row r="47" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T46" s="13"/>
+    </row>
+    <row r="47" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>433</v>
       </c>
@@ -13339,12 +13495,12 @@
       <c r="P47" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="Q47" s="13" t="s">
-        <v>1612</v>
-      </c>
-      <c r="R47" s="13"/>
-    </row>
-    <row r="48" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="R47" s="13" t="s">
+        <v>1598</v>
+      </c>
+      <c r="T47" s="13"/>
+    </row>
+    <row r="48" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>442</v>
       </c>
@@ -13374,9 +13530,9 @@
       <c r="P48" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="R48" s="13"/>
-    </row>
-    <row r="49" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T48" s="13"/>
+    </row>
+    <row r="49" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>447</v>
       </c>
@@ -13389,10 +13545,10 @@
         <v>1413</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>1711</v>
+        <v>1668</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>1710</v>
+        <v>1667</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
@@ -13406,9 +13562,9 @@
       <c r="P49" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R49" s="13"/>
-    </row>
-    <row r="50" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T49" s="13"/>
+    </row>
+    <row r="50" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>456</v>
       </c>
@@ -13437,9 +13593,9 @@
       <c r="P50" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R50" s="13"/>
-    </row>
-    <row r="51" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T50" s="13"/>
+    </row>
+    <row r="51" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>469</v>
       </c>
@@ -13474,9 +13630,9 @@
       <c r="P51" s="2" t="s">
         <v>1527</v>
       </c>
-      <c r="R51" s="13"/>
-    </row>
-    <row r="52" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T51" s="13"/>
+    </row>
+    <row r="52" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>476</v>
       </c>
@@ -13496,7 +13652,7 @@
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="14" t="s">
-        <v>1760</v>
+        <v>1717</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>1413</v>
@@ -13508,9 +13664,9 @@
       <c r="P52" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R52" s="13"/>
-    </row>
-    <row r="53" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+      <c r="T52" s="13"/>
+    </row>
+    <row r="53" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>482</v>
       </c>
@@ -13521,10 +13677,10 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>1713</v>
+        <v>1670</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>1712</v>
+        <v>1669</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>1438</v>
@@ -13540,14 +13696,20 @@
       <c r="P53" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="Q53" s="13" t="s">
-        <v>1613</v>
-      </c>
-      <c r="R53" s="13" t="s">
-        <v>1663</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q53" s="2" t="s">
+        <v>1789</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>1790</v>
+      </c>
+      <c r="S53" s="13" t="s">
+        <v>1784</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>492</v>
       </c>
@@ -13563,7 +13725,7 @@
         <v>493</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>1714</v>
+        <v>1671</v>
       </c>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
@@ -13582,9 +13744,9 @@
       <c r="P54" s="2" t="s">
         <v>1529</v>
       </c>
-      <c r="R54" s="13"/>
-    </row>
-    <row r="55" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T54" s="13"/>
+    </row>
+    <row r="55" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>498</v>
       </c>
@@ -13613,9 +13775,9 @@
       <c r="P55" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R55" s="13"/>
-    </row>
-    <row r="56" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T55" s="13"/>
+    </row>
+    <row r="56" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>499</v>
       </c>
@@ -13644,9 +13806,9 @@
       <c r="P56" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R56" s="13"/>
-    </row>
-    <row r="57" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T56" s="13"/>
+    </row>
+    <row r="57" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>500</v>
       </c>
@@ -13676,9 +13838,9 @@
       <c r="P57" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R57" s="13"/>
-    </row>
-    <row r="58" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T57" s="13"/>
+    </row>
+    <row r="58" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>505</v>
       </c>
@@ -13707,9 +13869,9 @@
       <c r="P58" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R58" s="13"/>
-    </row>
-    <row r="59" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T58" s="13"/>
+    </row>
+    <row r="59" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>506</v>
       </c>
@@ -13737,7 +13899,7 @@
         <v>1371</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>1790</v>
+        <v>1747</v>
       </c>
       <c r="O59" s="13" t="s">
         <v>1413</v>
@@ -13745,9 +13907,9 @@
       <c r="P59" s="2" t="s">
         <v>1530</v>
       </c>
-      <c r="R59" s="13"/>
-    </row>
-    <row r="60" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T59" s="13"/>
+    </row>
+    <row r="60" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>512</v>
       </c>
@@ -13776,9 +13938,9 @@
       <c r="P60" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R60" s="13"/>
-    </row>
-    <row r="61" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T60" s="13"/>
+    </row>
+    <row r="61" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>1367</v>
       </c>
@@ -13794,7 +13956,7 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="12" t="s">
-        <v>1715</v>
+        <v>1672</v>
       </c>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
@@ -13805,10 +13967,10 @@
         <v>1413</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>1792</v>
+        <v>1749</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>1791</v>
+        <v>1748</v>
       </c>
       <c r="O61" s="13" t="s">
         <v>1413</v>
@@ -13816,9 +13978,9 @@
       <c r="P61" s="2" t="s">
         <v>1531</v>
       </c>
-      <c r="R61" s="13"/>
-    </row>
-    <row r="62" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T61" s="13"/>
+    </row>
+    <row r="62" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
         <v>519</v>
       </c>
@@ -13847,9 +14009,9 @@
       <c r="P62" s="2" t="s">
         <v>1532</v>
       </c>
-      <c r="R62" s="13"/>
-    </row>
-    <row r="63" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T62" s="13"/>
+    </row>
+    <row r="63" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>1227</v>
       </c>
@@ -13878,9 +14040,9 @@
       <c r="P63" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R63" s="13"/>
-    </row>
-    <row r="64" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T63" s="13"/>
+    </row>
+    <row r="64" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>531</v>
       </c>
@@ -13913,14 +14075,20 @@
       <c r="P64" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="Q64" s="13" t="s">
-        <v>1614</v>
-      </c>
-      <c r="R64" s="13" t="s">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="Q64" s="2" t="s">
+        <v>1785</v>
+      </c>
+      <c r="R64" s="2" t="s">
+        <v>1770</v>
+      </c>
+      <c r="S64" s="13" t="s">
+        <v>533</v>
+      </c>
+      <c r="T64" s="13" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>538</v>
       </c>
@@ -13935,7 +14103,7 @@
         <v>1413</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>1716</v>
+        <v>1673</v>
       </c>
       <c r="G65" s="12" t="s">
         <v>294</v>
@@ -13947,24 +14115,27 @@
         <v>1450</v>
       </c>
       <c r="K65" s="14" t="s">
-        <v>1770</v>
+        <v>1727</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>1771</v>
+        <v>1728</v>
       </c>
       <c r="N65" s="13"/>
       <c r="O65" s="13"/>
       <c r="P65" s="2" t="s">
         <v>1534</v>
       </c>
-      <c r="Q65" s="13" t="s">
-        <v>1615</v>
-      </c>
-      <c r="R65" s="13" t="s">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q65" s="2" t="s">
+        <v>1786</v>
+      </c>
+      <c r="S65" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="T65" s="13" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>546</v>
       </c>
@@ -13992,9 +14163,9 @@
       <c r="P66" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="R66" s="13"/>
-    </row>
-    <row r="67" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T66" s="13"/>
+    </row>
+    <row r="67" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>549</v>
       </c>
@@ -14024,9 +14195,9 @@
       <c r="P67" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R67" s="13"/>
-    </row>
-    <row r="68" spans="1:18" ht="170" x14ac:dyDescent="0.2">
+      <c r="T67" s="13"/>
+    </row>
+    <row r="68" spans="1:20" ht="170" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>552</v>
       </c>
@@ -14053,14 +14224,20 @@
       <c r="P68" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="Q68" s="13" t="s">
-        <v>1616</v>
-      </c>
-      <c r="R68" s="13" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q68" s="2" t="s">
+        <v>1787</v>
+      </c>
+      <c r="R68" s="2" t="s">
+        <v>1788</v>
+      </c>
+      <c r="S68" s="13" t="s">
+        <v>1734</v>
+      </c>
+      <c r="T68" s="13" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>559</v>
       </c>
@@ -14090,14 +14267,14 @@
       <c r="P69" s="2" t="s">
         <v>1535</v>
       </c>
-      <c r="Q69" s="13" t="s">
+      <c r="S69" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="R69" s="13" t="s">
-        <v>1667</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T69" s="13" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>563</v>
       </c>
@@ -14127,11 +14304,11 @@
       <c r="P70" s="2" t="s">
         <v>1536</v>
       </c>
-      <c r="R70" s="13" t="s">
-        <v>1668</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T70" s="13" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>567</v>
       </c>
@@ -14161,9 +14338,9 @@
       <c r="P71" s="2" t="s">
         <v>1537</v>
       </c>
-      <c r="R71" s="13"/>
-    </row>
-    <row r="72" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T71" s="13"/>
+    </row>
+    <row r="72" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
         <v>576</v>
       </c>
@@ -14192,9 +14369,9 @@
       <c r="P72" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R72" s="13"/>
-    </row>
-    <row r="73" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T72" s="13"/>
+    </row>
+    <row r="73" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
         <v>577</v>
       </c>
@@ -14225,12 +14402,15 @@
       <c r="P73" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="Q73" s="13" t="s">
-        <v>1617</v>
-      </c>
-      <c r="R73" s="13"/>
-    </row>
-    <row r="74" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q73" s="2" t="s">
+        <v>1791</v>
+      </c>
+      <c r="S73" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="T73" s="13"/>
+    </row>
+    <row r="74" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>581</v>
       </c>
@@ -14259,9 +14439,9 @@
       <c r="P74" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R74" s="13"/>
-    </row>
-    <row r="75" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T74" s="13"/>
+    </row>
+    <row r="75" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
         <v>582</v>
       </c>
@@ -14290,9 +14470,9 @@
       <c r="P75" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R75" s="13"/>
-    </row>
-    <row r="76" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T75" s="13"/>
+    </row>
+    <row r="76" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
         <v>583</v>
       </c>
@@ -14323,9 +14503,9 @@
       <c r="P76" s="2" t="s">
         <v>1539</v>
       </c>
-      <c r="R76" s="13"/>
-    </row>
-    <row r="77" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T76" s="13"/>
+    </row>
+    <row r="77" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
         <v>587</v>
       </c>
@@ -14354,9 +14534,9 @@
       <c r="P77" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="R77" s="13"/>
-    </row>
-    <row r="78" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T77" s="13"/>
+    </row>
+    <row r="78" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>593</v>
       </c>
@@ -14387,9 +14567,9 @@
       <c r="P78" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R78" s="13"/>
-    </row>
-    <row r="79" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T78" s="13"/>
+    </row>
+    <row r="79" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>596</v>
       </c>
@@ -14418,9 +14598,9 @@
       <c r="P79" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R79" s="13"/>
-    </row>
-    <row r="80" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T79" s="13"/>
+    </row>
+    <row r="80" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
         <v>597</v>
       </c>
@@ -14449,9 +14629,9 @@
       <c r="P80" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R80" s="13"/>
-    </row>
-    <row r="81" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T80" s="13"/>
+    </row>
+    <row r="81" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>598</v>
       </c>
@@ -14473,10 +14653,10 @@
         <v>1413</v>
       </c>
       <c r="K81" s="14" t="s">
-        <v>1773</v>
+        <v>1730</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>1772</v>
+        <v>1729</v>
       </c>
       <c r="N81" s="13"/>
       <c r="O81" s="13" t="s">
@@ -14485,12 +14665,15 @@
       <c r="P81" s="2" t="s">
         <v>1541</v>
       </c>
-      <c r="Q81" s="13" t="s">
-        <v>1618</v>
-      </c>
-      <c r="R81" s="13"/>
-    </row>
-    <row r="82" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q81" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="S81" s="13" t="s">
+        <v>1793</v>
+      </c>
+      <c r="T81" s="13"/>
+    </row>
+    <row r="82" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
         <v>605</v>
       </c>
@@ -14521,9 +14704,9 @@
       <c r="P82" s="2" t="s">
         <v>1542</v>
       </c>
-      <c r="R82" s="13"/>
-    </row>
-    <row r="83" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T82" s="13"/>
+    </row>
+    <row r="83" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
         <v>610</v>
       </c>
@@ -14554,9 +14737,9 @@
       <c r="P83" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="R83" s="13"/>
-    </row>
-    <row r="84" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T83" s="13"/>
+    </row>
+    <row r="84" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
         <v>618</v>
       </c>
@@ -14589,14 +14772,17 @@
       <c r="P84" s="2" t="s">
         <v>1543</v>
       </c>
-      <c r="Q84" s="13" t="s">
-        <v>1619</v>
-      </c>
-      <c r="R84" s="13" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="Q84" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="S84" s="13" t="s">
+        <v>1794</v>
+      </c>
+      <c r="T84" s="13" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
         <v>627</v>
       </c>
@@ -14628,14 +14814,17 @@
       <c r="P85" s="2" t="s">
         <v>1544</v>
       </c>
-      <c r="Q85" s="13" t="s">
-        <v>1620</v>
-      </c>
-      <c r="R85" s="13" t="s">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q85" s="2" t="s">
+        <v>1796</v>
+      </c>
+      <c r="S85" s="13" t="s">
+        <v>1795</v>
+      </c>
+      <c r="T85" s="13" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
         <v>633</v>
       </c>
@@ -14667,14 +14856,17 @@
       <c r="P86" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="Q86" s="13" t="s">
-        <v>1621</v>
-      </c>
-      <c r="R86" s="13" t="s">
-        <v>1671</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="R86" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="S86" s="13" t="s">
+        <v>1797</v>
+      </c>
+      <c r="T86" s="13" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
         <v>639</v>
       </c>
@@ -14687,10 +14879,10 @@
         <v>2015</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>1718</v>
+        <v>1675</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>1717</v>
+        <v>1674</v>
       </c>
       <c r="H87" s="13" t="s">
         <v>160</v>
@@ -14708,14 +14900,17 @@
       <c r="P87" s="2" t="s">
         <v>1545</v>
       </c>
-      <c r="Q87" s="13" t="s">
-        <v>1622</v>
-      </c>
-      <c r="R87" s="13" t="s">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R87" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="S87" s="13" t="s">
+        <v>1799</v>
+      </c>
+      <c r="T87" s="13" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
         <v>650</v>
       </c>
@@ -14744,9 +14939,9 @@
       <c r="P88" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R88" s="13"/>
-    </row>
-    <row r="89" spans="1:18" ht="289" x14ac:dyDescent="0.2">
+      <c r="T88" s="13"/>
+    </row>
+    <row r="89" spans="1:20" ht="289" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>160</v>
       </c>
@@ -14761,10 +14956,10 @@
         <v>1413</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1719</v>
+        <v>1676</v>
       </c>
       <c r="G89" s="12" t="s">
-        <v>1699</v>
+        <v>1656</v>
       </c>
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
@@ -14778,12 +14973,18 @@
       <c r="P89" s="2" t="s">
         <v>1546</v>
       </c>
-      <c r="Q89" s="13" t="s">
-        <v>1623</v>
-      </c>
-      <c r="R89" s="13"/>
-    </row>
-    <row r="90" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q89" s="2" t="s">
+        <v>1800</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="S89" s="13" t="s">
+        <v>1801</v>
+      </c>
+      <c r="T89" s="13"/>
+    </row>
+    <row r="90" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
         <v>1264</v>
       </c>
@@ -14814,14 +15015,17 @@
       <c r="P90" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="Q90" s="13" t="s">
-        <v>1624</v>
-      </c>
-      <c r="R90" s="13" t="s">
+      <c r="R90" s="2" t="s">
+        <v>1803</v>
+      </c>
+      <c r="S90" s="13" t="s">
+        <v>1802</v>
+      </c>
+      <c r="T90" s="13" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
         <v>1266</v>
       </c>
@@ -14839,7 +15043,7 @@
         <v>470</v>
       </c>
       <c r="G91" s="12" t="s">
-        <v>1720</v>
+        <v>1677</v>
       </c>
       <c r="H91" s="13" t="s">
         <v>160</v>
@@ -14855,14 +15059,17 @@
       <c r="P91" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="Q91" s="13" t="s">
-        <v>1625</v>
-      </c>
-      <c r="R91" s="13" t="s">
-        <v>1673</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q91" s="2" t="s">
+        <v>1805</v>
+      </c>
+      <c r="S91" s="13" t="s">
+        <v>1804</v>
+      </c>
+      <c r="T91" s="13" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
         <v>669</v>
       </c>
@@ -14875,7 +15082,7 @@
         <v>1413</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>1721</v>
+        <v>1678</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>671</v>
@@ -14893,12 +15100,15 @@
       <c r="P92" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="Q92" s="13" t="s">
-        <v>1626</v>
-      </c>
-      <c r="R92" s="13"/>
-    </row>
-    <row r="93" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q92" s="2" t="s">
+        <v>1807</v>
+      </c>
+      <c r="S92" s="13" t="s">
+        <v>1806</v>
+      </c>
+      <c r="T92" s="13"/>
+    </row>
+    <row r="93" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>1270</v>
       </c>
@@ -14928,14 +15138,17 @@
       <c r="P93" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="Q93" s="13" t="s">
-        <v>1627</v>
-      </c>
-      <c r="R93" s="13" t="s">
+      <c r="Q93" s="2" t="s">
+        <v>1808</v>
+      </c>
+      <c r="S93" s="13" t="s">
+        <v>1423</v>
+      </c>
+      <c r="T93" s="13" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
         <v>680</v>
       </c>
@@ -14948,7 +15161,7 @@
         <v>1413</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>1722</v>
+        <v>1679</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>550</v>
@@ -14968,9 +15181,9 @@
       <c r="P94" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="R94" s="13"/>
-    </row>
-    <row r="95" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T94" s="13"/>
+    </row>
+    <row r="95" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>683</v>
       </c>
@@ -15003,14 +15216,14 @@
       <c r="P95" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="Q95" s="13" t="s">
+      <c r="R95" s="13" t="s">
         <v>686</v>
       </c>
-      <c r="R95" s="13" t="s">
-        <v>1674</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T95" s="13" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
         <v>689</v>
       </c>
@@ -15023,7 +15236,7 @@
         <v>1413</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>1723</v>
+        <v>1680</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>533</v>
@@ -15042,14 +15255,17 @@
       <c r="P96" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="Q96" s="13" t="s">
-        <v>1628</v>
-      </c>
-      <c r="R96" s="13" t="s">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R96" s="2" t="s">
+        <v>1765</v>
+      </c>
+      <c r="S96" s="13" t="s">
+        <v>533</v>
+      </c>
+      <c r="T96" s="13" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
         <v>696</v>
       </c>
@@ -15081,12 +15297,12 @@
       <c r="P97" s="2" t="s">
         <v>1548</v>
       </c>
-      <c r="Q97" s="13" t="s">
-        <v>1629</v>
-      </c>
-      <c r="R97" s="13"/>
-    </row>
-    <row r="98" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S97" s="13" t="s">
+        <v>1599</v>
+      </c>
+      <c r="T97" s="13"/>
+    </row>
+    <row r="98" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
         <v>704</v>
       </c>
@@ -15115,9 +15331,9 @@
       <c r="P98" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R98" s="13"/>
-    </row>
-    <row r="99" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T98" s="13"/>
+    </row>
+    <row r="99" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>705</v>
       </c>
@@ -15132,7 +15348,7 @@
         <v>1413</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>1724</v>
+        <v>1681</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>533</v>
@@ -15152,14 +15368,14 @@
       <c r="P99" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q99" s="13" t="s">
-        <v>1630</v>
-      </c>
-      <c r="R99" s="13" t="s">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S99" s="13" t="s">
+        <v>1600</v>
+      </c>
+      <c r="T99" s="13" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
         <v>712</v>
       </c>
@@ -15188,9 +15404,9 @@
       <c r="P100" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R100" s="13"/>
-    </row>
-    <row r="101" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T100" s="13"/>
+    </row>
+    <row r="101" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
         <v>713</v>
       </c>
@@ -15219,9 +15435,9 @@
       <c r="P101" s="2" t="s">
         <v>1549</v>
       </c>
-      <c r="R101" s="13"/>
-    </row>
-    <row r="102" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T101" s="13"/>
+    </row>
+    <row r="102" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
         <v>722</v>
       </c>
@@ -15234,10 +15450,10 @@
         <v>1413</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>1726</v>
+        <v>1683</v>
       </c>
       <c r="G102" s="12" t="s">
-        <v>1725</v>
+        <v>1682</v>
       </c>
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
@@ -15254,12 +15470,12 @@
       <c r="P102" s="2" t="s">
         <v>1550</v>
       </c>
-      <c r="Q102" s="13" t="s">
-        <v>1631</v>
-      </c>
-      <c r="R102" s="13"/>
-    </row>
-    <row r="103" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S102" s="13" t="s">
+        <v>1601</v>
+      </c>
+      <c r="T102" s="13"/>
+    </row>
+    <row r="103" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
         <v>728</v>
       </c>
@@ -15288,9 +15504,9 @@
       <c r="P103" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R103" s="13"/>
-    </row>
-    <row r="104" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+      <c r="T103" s="13"/>
+    </row>
+    <row r="104" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
         <v>729</v>
       </c>
@@ -15305,7 +15521,7 @@
         <v>2017</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>1727</v>
+        <v>1684</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>1425</v>
@@ -15324,14 +15540,17 @@
       <c r="P104" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="Q104" s="13" t="s">
-        <v>1632</v>
-      </c>
-      <c r="R104" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q104" s="2" t="s">
+        <v>1810</v>
+      </c>
+      <c r="S104" s="13" t="s">
+        <v>1809</v>
+      </c>
+      <c r="T104" s="13" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
         <v>1286</v>
       </c>
@@ -15363,12 +15582,15 @@
       <c r="P105" s="2" t="s">
         <v>1551</v>
       </c>
-      <c r="Q105" s="13" t="s">
-        <v>1633</v>
-      </c>
-      <c r="R105" s="13"/>
-    </row>
-    <row r="106" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R105" s="2" t="s">
+        <v>1811</v>
+      </c>
+      <c r="S105" s="13" t="s">
+        <v>1812</v>
+      </c>
+      <c r="T105" s="13"/>
+    </row>
+    <row r="106" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
         <v>743</v>
       </c>
@@ -15397,9 +15619,9 @@
       <c r="P106" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R106" s="13"/>
-    </row>
-    <row r="107" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T106" s="13"/>
+    </row>
+    <row r="107" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>744</v>
       </c>
@@ -15428,9 +15650,9 @@
       <c r="P107" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R107" s="13"/>
-    </row>
-    <row r="108" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+      <c r="T107" s="13"/>
+    </row>
+    <row r="108" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
         <v>745</v>
       </c>
@@ -15446,7 +15668,7 @@
         <v>747</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>1728</v>
+        <v>1685</v>
       </c>
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
@@ -15460,9 +15682,9 @@
       <c r="P108" s="2" t="s">
         <v>1552</v>
       </c>
-      <c r="R108" s="13"/>
-    </row>
-    <row r="109" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T108" s="13"/>
+    </row>
+    <row r="109" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
         <v>755</v>
       </c>
@@ -15490,14 +15712,17 @@
       <c r="P109" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q109" s="13" t="s">
-        <v>1634</v>
+      <c r="Q109" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="R109" s="13" t="s">
-        <v>1678</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+        <v>1813</v>
+      </c>
+      <c r="T109" s="13" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
         <v>759</v>
       </c>
@@ -15526,9 +15751,9 @@
       <c r="P110" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R110" s="13"/>
-    </row>
-    <row r="111" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="T110" s="13"/>
+    </row>
+    <row r="111" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
         <v>760</v>
       </c>
@@ -15549,10 +15774,10 @@
       </c>
       <c r="I111" s="13"/>
       <c r="K111" s="14" t="s">
-        <v>1775</v>
+        <v>1732</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>1774</v>
+        <v>1731</v>
       </c>
       <c r="N111" s="13"/>
       <c r="O111" s="13" t="s">
@@ -15561,14 +15786,17 @@
       <c r="P111" s="2" t="s">
         <v>1553</v>
       </c>
-      <c r="Q111" s="13" t="s">
-        <v>1635</v>
-      </c>
-      <c r="R111" s="13" t="s">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q111" s="2" t="s">
+        <v>1815</v>
+      </c>
+      <c r="S111" s="13" t="s">
+        <v>1814</v>
+      </c>
+      <c r="T111" s="13" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
         <v>769</v>
       </c>
@@ -15598,9 +15826,9 @@
       <c r="P112" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R112" s="13"/>
-    </row>
-    <row r="113" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T112" s="13"/>
+    </row>
+    <row r="113" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
         <v>772</v>
       </c>
@@ -15633,9 +15861,9 @@
       <c r="P113" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="R113" s="13"/>
-    </row>
-    <row r="114" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T113" s="13"/>
+    </row>
+    <row r="114" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
         <v>780</v>
       </c>
@@ -15664,9 +15892,9 @@
       <c r="P114" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R114" s="13"/>
-    </row>
-    <row r="115" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T114" s="13"/>
+    </row>
+    <row r="115" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>781</v>
       </c>
@@ -15697,9 +15925,9 @@
       <c r="P115" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R115" s="13"/>
-    </row>
-    <row r="116" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+      <c r="T115" s="13"/>
+    </row>
+    <row r="116" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
         <v>792</v>
       </c>
@@ -15728,9 +15956,9 @@
       <c r="P116" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R116" s="13"/>
-    </row>
-    <row r="117" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T116" s="13"/>
+    </row>
+    <row r="117" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
         <v>796</v>
       </c>
@@ -15762,9 +15990,9 @@
       <c r="P117" s="2" t="s">
         <v>1554</v>
       </c>
-      <c r="R117" s="13"/>
-    </row>
-    <row r="118" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T117" s="13"/>
+    </row>
+    <row r="118" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
         <v>802</v>
       </c>
@@ -15795,14 +16023,14 @@
       <c r="P118" s="2" t="s">
         <v>1554</v>
       </c>
-      <c r="Q118" s="13" t="s">
+      <c r="S118" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="R118" s="13" t="s">
+      <c r="T118" s="13" t="s">
         <v>1295</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
         <v>806</v>
       </c>
@@ -15831,9 +16059,9 @@
       <c r="P119" s="2" t="s">
         <v>1555</v>
       </c>
-      <c r="R119" s="13"/>
-    </row>
-    <row r="120" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T119" s="13"/>
+    </row>
+    <row r="120" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
         <v>814</v>
       </c>
@@ -15846,10 +16074,10 @@
         <v>1413</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>1730</v>
+        <v>1687</v>
       </c>
       <c r="G120" s="12" t="s">
-        <v>1729</v>
+        <v>1686</v>
       </c>
       <c r="H120" s="13"/>
       <c r="I120" s="13"/>
@@ -15863,7 +16091,7 @@
         <v>1371</v>
       </c>
       <c r="N120" s="13" t="s">
-        <v>1793</v>
+        <v>1750</v>
       </c>
       <c r="O120" s="13" t="s">
         <v>1413</v>
@@ -15871,9 +16099,9 @@
       <c r="P120" s="2" t="s">
         <v>1556</v>
       </c>
-      <c r="R120" s="13"/>
-    </row>
-    <row r="121" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T120" s="13"/>
+    </row>
+    <row r="121" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
         <v>824</v>
       </c>
@@ -15901,7 +16129,7 @@
         <v>1371</v>
       </c>
       <c r="N121" s="13" t="s">
-        <v>1794</v>
+        <v>1751</v>
       </c>
       <c r="O121" s="13" t="s">
         <v>1413</v>
@@ -15909,9 +16137,9 @@
       <c r="P121" s="2" t="s">
         <v>1557</v>
       </c>
-      <c r="R121" s="13"/>
-    </row>
-    <row r="122" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T121" s="13"/>
+    </row>
+    <row r="122" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>832</v>
       </c>
@@ -15942,9 +16170,9 @@
       <c r="P122" s="2" t="s">
         <v>1558</v>
       </c>
-      <c r="R122" s="13"/>
-    </row>
-    <row r="123" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T122" s="13"/>
+    </row>
+    <row r="123" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>840</v>
       </c>
@@ -15972,7 +16200,7 @@
         <v>1485</v>
       </c>
       <c r="N123" s="13" t="s">
-        <v>1795</v>
+        <v>1752</v>
       </c>
       <c r="O123" s="13" t="s">
         <v>1413</v>
@@ -15980,9 +16208,9 @@
       <c r="P123" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="R123" s="13"/>
-    </row>
-    <row r="124" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T123" s="13"/>
+    </row>
+    <row r="124" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
         <v>845</v>
       </c>
@@ -15997,7 +16225,7 @@
         <v>2005</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>1731</v>
+        <v>1688</v>
       </c>
       <c r="G124" s="12" t="s">
         <v>445</v>
@@ -16018,11 +16246,14 @@
         <v>849</v>
       </c>
       <c r="Q124" s="13" t="s">
-        <v>1636</v>
-      </c>
-      <c r="R124" s="13"/>
-    </row>
-    <row r="125" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+        <v>1816</v>
+      </c>
+      <c r="R124" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="T124" s="13"/>
+    </row>
+    <row r="125" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
         <v>853</v>
       </c>
@@ -16051,9 +16282,9 @@
       <c r="P125" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R125" s="13"/>
-    </row>
-    <row r="126" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T125" s="13"/>
+    </row>
+    <row r="126" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
         <v>865</v>
       </c>
@@ -16082,9 +16313,9 @@
       <c r="P126" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R126" s="13"/>
-    </row>
-    <row r="127" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T126" s="13"/>
+    </row>
+    <row r="127" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
         <v>866</v>
       </c>
@@ -16113,9 +16344,9 @@
       <c r="P127" s="2" t="s">
         <v>1559</v>
       </c>
-      <c r="R127" s="13"/>
-    </row>
-    <row r="128" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T127" s="13"/>
+    </row>
+    <row r="128" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>1302</v>
       </c>
@@ -16144,9 +16375,9 @@
       <c r="P128" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R128" s="13"/>
-    </row>
-    <row r="129" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T128" s="13"/>
+    </row>
+    <row r="129" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>869</v>
       </c>
@@ -16159,10 +16390,10 @@
         <v>1413</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>1733</v>
+        <v>1690</v>
       </c>
       <c r="G129" s="12" t="s">
-        <v>1732</v>
+        <v>1689</v>
       </c>
       <c r="H129" s="13"/>
       <c r="I129" s="13"/>
@@ -16179,12 +16410,12 @@
       <c r="P129" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="Q129" s="13" t="s">
-        <v>1637</v>
-      </c>
-      <c r="R129" s="13"/>
-    </row>
-    <row r="130" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S129" s="13" t="s">
+        <v>1602</v>
+      </c>
+      <c r="T129" s="13"/>
+    </row>
+    <row r="130" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
         <v>872</v>
       </c>
@@ -16217,11 +16448,11 @@
       <c r="P130" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R130" s="13" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T130" s="13" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>878</v>
       </c>
@@ -16234,10 +16465,10 @@
         <v>1413</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>1735</v>
+        <v>1692</v>
       </c>
       <c r="G131" s="12" t="s">
-        <v>1734</v>
+        <v>1691</v>
       </c>
       <c r="H131" s="13" t="s">
         <v>160</v>
@@ -16253,12 +16484,12 @@
       <c r="P131" s="2" t="s">
         <v>1503</v>
       </c>
-      <c r="Q131" s="13" t="s">
-        <v>1638</v>
-      </c>
-      <c r="R131" s="13"/>
-    </row>
-    <row r="132" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S131" s="13" t="s">
+        <v>1603</v>
+      </c>
+      <c r="T131" s="13"/>
+    </row>
+    <row r="132" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>884</v>
       </c>
@@ -16287,12 +16518,15 @@
       <c r="P132" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q132" s="13" t="s">
-        <v>1639</v>
-      </c>
-      <c r="R132" s="13"/>
-    </row>
-    <row r="133" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q132" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="S132" s="13" t="s">
+        <v>1818</v>
+      </c>
+      <c r="T132" s="13"/>
+    </row>
+    <row r="133" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>890</v>
       </c>
@@ -16323,9 +16557,9 @@
       <c r="P133" s="2" t="s">
         <v>1560</v>
       </c>
-      <c r="R133" s="13"/>
-    </row>
-    <row r="134" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T133" s="13"/>
+    </row>
+    <row r="134" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>897</v>
       </c>
@@ -16354,9 +16588,9 @@
       <c r="P134" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R134" s="13"/>
-    </row>
-    <row r="135" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T134" s="13"/>
+    </row>
+    <row r="135" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>898</v>
       </c>
@@ -16371,10 +16605,10 @@
         <v>1413</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>1737</v>
+        <v>1694</v>
       </c>
       <c r="G135" s="12" t="s">
-        <v>1736</v>
+        <v>1693</v>
       </c>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
@@ -16391,14 +16625,14 @@
       <c r="P135" s="2" t="s">
         <v>1561</v>
       </c>
-      <c r="Q135" s="13" t="s">
-        <v>1640</v>
-      </c>
-      <c r="R135" s="13" t="s">
+      <c r="S135" s="13" t="s">
+        <v>1604</v>
+      </c>
+      <c r="T135" s="13" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
         <v>913</v>
       </c>
@@ -16427,9 +16661,9 @@
       <c r="P136" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R136" s="13"/>
-    </row>
-    <row r="137" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T136" s="13"/>
+    </row>
+    <row r="137" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>914</v>
       </c>
@@ -16442,7 +16676,7 @@
         <v>1413</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>1600</v>
+        <v>1592</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>611</v>
@@ -16462,12 +16696,12 @@
       <c r="P137" s="2" t="s">
         <v>1562</v>
       </c>
-      <c r="Q137" s="13" t="s">
-        <v>1600</v>
-      </c>
-      <c r="R137" s="13"/>
-    </row>
-    <row r="138" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="S137" s="13" t="s">
+        <v>1592</v>
+      </c>
+      <c r="T137" s="13"/>
+    </row>
+    <row r="138" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>918</v>
       </c>
@@ -16497,9 +16731,9 @@
       <c r="P138" s="2" t="s">
         <v>1563</v>
       </c>
-      <c r="R138" s="13"/>
-    </row>
-    <row r="139" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T138" s="13"/>
+    </row>
+    <row r="139" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>923</v>
       </c>
@@ -16512,10 +16746,10 @@
         <v>1413</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>1739</v>
+        <v>1696</v>
       </c>
       <c r="G139" s="12" t="s">
-        <v>1738</v>
+        <v>1695</v>
       </c>
       <c r="H139" s="13"/>
       <c r="I139" s="14" t="s">
@@ -16531,9 +16765,9 @@
       <c r="P139" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="R139" s="13"/>
-    </row>
-    <row r="140" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T139" s="13"/>
+    </row>
+    <row r="140" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>929</v>
       </c>
@@ -16559,7 +16793,7 @@
         <v>1371</v>
       </c>
       <c r="N140" s="13" t="s">
-        <v>1796</v>
+        <v>1753</v>
       </c>
       <c r="O140" s="13" t="s">
         <v>1413</v>
@@ -16567,9 +16801,9 @@
       <c r="P140" s="2" t="s">
         <v>1564</v>
       </c>
-      <c r="R140" s="13"/>
-    </row>
-    <row r="141" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T140" s="13"/>
+    </row>
+    <row r="141" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="10" t="s">
         <v>1309</v>
       </c>
@@ -16597,9 +16831,9 @@
       <c r="P141" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R141" s="13"/>
-    </row>
-    <row r="142" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T141" s="13"/>
+    </row>
+    <row r="142" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A142" s="10" t="s">
         <v>935</v>
       </c>
@@ -16627,9 +16861,9 @@
       <c r="P142" s="2" t="s">
         <v>1565</v>
       </c>
-      <c r="R142" s="13"/>
-    </row>
-    <row r="143" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T142" s="13"/>
+    </row>
+    <row r="143" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="10" t="s">
         <v>942</v>
       </c>
@@ -16661,12 +16895,12 @@
       <c r="P143" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="Q143" s="13" t="s">
-        <v>1641</v>
-      </c>
-      <c r="R143" s="13"/>
-    </row>
-    <row r="144" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="S143" s="13" t="s">
+        <v>1605</v>
+      </c>
+      <c r="T143" s="13"/>
+    </row>
+    <row r="144" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>947</v>
       </c>
@@ -16681,10 +16915,10 @@
         <v>1413</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>1741</v>
+        <v>1698</v>
       </c>
       <c r="G144" s="12" t="s">
-        <v>1740</v>
+        <v>1697</v>
       </c>
       <c r="H144" s="13"/>
       <c r="I144" s="14" t="s">
@@ -16700,9 +16934,9 @@
       <c r="P144" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="R144" s="13"/>
-    </row>
-    <row r="145" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T144" s="13"/>
+    </row>
+    <row r="145" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
         <v>956</v>
       </c>
@@ -16730,9 +16964,9 @@
       <c r="P145" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R145" s="13"/>
-    </row>
-    <row r="146" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="T145" s="13"/>
+    </row>
+    <row r="146" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A146" s="10" t="s">
         <v>957</v>
       </c>
@@ -16760,9 +16994,9 @@
       <c r="P146" s="2" t="s">
         <v>1566</v>
       </c>
-      <c r="R146" s="13"/>
-    </row>
-    <row r="147" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T146" s="13"/>
+    </row>
+    <row r="147" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="10" t="s">
         <v>1313</v>
       </c>
@@ -16775,7 +17009,7 @@
         <v>1413</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>1742</v>
+        <v>1699</v>
       </c>
       <c r="G147" s="12" t="s">
         <v>1425</v>
@@ -16795,9 +17029,9 @@
       <c r="P147" s="2" t="s">
         <v>1567</v>
       </c>
-      <c r="R147" s="13"/>
-    </row>
-    <row r="148" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T147" s="13"/>
+    </row>
+    <row r="148" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>970</v>
       </c>
@@ -16814,20 +17048,20 @@
         <v>2014</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>1743</v>
+        <v>1700</v>
       </c>
       <c r="G148" s="12" t="s">
-        <v>1699</v>
+        <v>1656</v>
       </c>
       <c r="H148" s="13" t="s">
         <v>765</v>
       </c>
       <c r="I148" s="13"/>
       <c r="K148" s="14" t="s">
-        <v>1777</v>
+        <v>1734</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>1776</v>
+        <v>1733</v>
       </c>
       <c r="N148" s="13"/>
       <c r="O148" s="13" t="s">
@@ -16836,14 +17070,17 @@
       <c r="P148" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q148" s="13" t="s">
-        <v>1642</v>
-      </c>
-      <c r="R148" s="13" t="s">
-        <v>1681</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q148" s="2" t="s">
+        <v>1820</v>
+      </c>
+      <c r="S148" s="13" t="s">
+        <v>1819</v>
+      </c>
+      <c r="T148" s="13" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A149" s="10" t="s">
         <v>441</v>
       </c>
@@ -16858,7 +17095,7 @@
         <v>1998</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>1744</v>
+        <v>1701</v>
       </c>
       <c r="G149" s="12" t="s">
         <v>445</v>
@@ -16878,12 +17115,18 @@
       <c r="P149" s="2" t="s">
         <v>1568</v>
       </c>
-      <c r="Q149" s="13" t="s">
-        <v>1643</v>
-      </c>
-      <c r="R149" s="13"/>
-    </row>
-    <row r="150" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="Q149" s="2" t="s">
+        <v>1821</v>
+      </c>
+      <c r="R149" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="S149" s="13" t="s">
+        <v>1795</v>
+      </c>
+      <c r="T149" s="13"/>
+    </row>
+    <row r="150" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A150" s="10" t="s">
         <v>985</v>
       </c>
@@ -16914,11 +17157,11 @@
       <c r="P150" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R150" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T150" s="13" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A151" s="10" t="s">
         <v>992</v>
       </c>
@@ -16934,7 +17177,7 @@
         <v>628</v>
       </c>
       <c r="G151" s="12" t="s">
-        <v>1745</v>
+        <v>1702</v>
       </c>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
@@ -16951,12 +17194,15 @@
       <c r="P151" s="2" t="s">
         <v>1569</v>
       </c>
-      <c r="Q151" s="13" t="s">
-        <v>1644</v>
-      </c>
-      <c r="R151" s="13"/>
-    </row>
-    <row r="152" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q151" s="2" t="s">
+        <v>1823</v>
+      </c>
+      <c r="R151" s="13" t="s">
+        <v>1822</v>
+      </c>
+      <c r="T151" s="13"/>
+    </row>
+    <row r="152" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="10" t="s">
         <v>998</v>
       </c>
@@ -16969,7 +17215,7 @@
         <v>2009</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>1746</v>
+        <v>1703</v>
       </c>
       <c r="G152" s="12" t="s">
         <v>445</v>
@@ -16992,9 +17238,9 @@
       <c r="Q152" s="13" t="s">
         <v>1003</v>
       </c>
-      <c r="R152" s="13"/>
-    </row>
-    <row r="153" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T152" s="13"/>
+    </row>
+    <row r="153" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="10" t="s">
         <v>1005</v>
       </c>
@@ -17024,9 +17270,9 @@
       <c r="P153" s="2" t="s">
         <v>849</v>
       </c>
-      <c r="R153" s="13"/>
-    </row>
-    <row r="154" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T153" s="13"/>
+    </row>
+    <row r="154" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A154" s="10" t="s">
         <v>1007</v>
       </c>
@@ -17039,10 +17285,10 @@
         <v>2017</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>1748</v>
+        <v>1705</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>1747</v>
+        <v>1704</v>
       </c>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
@@ -17059,12 +17305,12 @@
       <c r="P154" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="Q154" s="13" t="s">
-        <v>1645</v>
-      </c>
-      <c r="R154" s="13"/>
-    </row>
-    <row r="155" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="S154" s="13" t="s">
+        <v>1606</v>
+      </c>
+      <c r="T154" s="13"/>
+    </row>
+    <row r="155" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A155" s="10" t="s">
         <v>1012</v>
       </c>
@@ -17095,9 +17341,9 @@
       <c r="P155" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="R155" s="13"/>
-    </row>
-    <row r="156" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T155" s="13"/>
+    </row>
+    <row r="156" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A156" s="10" t="s">
         <v>1017</v>
       </c>
@@ -17112,7 +17358,7 @@
         <v>1413</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>1749</v>
+        <v>1706</v>
       </c>
       <c r="G156" s="12" t="s">
         <v>507</v>
@@ -17132,14 +17378,14 @@
       <c r="P156" s="2" t="s">
         <v>1573</v>
       </c>
-      <c r="Q156" s="13" t="s">
+      <c r="S156" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="R156" s="13" t="s">
+      <c r="T156" s="13" t="s">
         <v>1295</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A157" s="10" t="s">
         <v>1021</v>
       </c>
@@ -17167,9 +17413,9 @@
       <c r="P157" s="2" t="s">
         <v>1574</v>
       </c>
-      <c r="R157" s="13"/>
-    </row>
-    <row r="158" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T157" s="13"/>
+    </row>
+    <row r="158" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A158" s="10" t="s">
         <v>1029</v>
       </c>
@@ -17200,9 +17446,9 @@
       <c r="P158" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="R158" s="13"/>
-    </row>
-    <row r="159" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T158" s="13"/>
+    </row>
+    <row r="159" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A159" s="10" t="s">
         <v>1034</v>
       </c>
@@ -17233,9 +17479,9 @@
       <c r="P159" s="2" t="s">
         <v>1576</v>
       </c>
-      <c r="R159" s="13"/>
-    </row>
-    <row r="160" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T159" s="13"/>
+    </row>
+    <row r="160" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
         <v>1039</v>
       </c>
@@ -17264,9 +17510,9 @@
       <c r="P160" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R160" s="13"/>
-    </row>
-    <row r="161" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T160" s="13"/>
+    </row>
+    <row r="161" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>1040</v>
       </c>
@@ -17295,9 +17541,9 @@
       <c r="P161" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R161" s="13"/>
-    </row>
-    <row r="162" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T161" s="13"/>
+    </row>
+    <row r="162" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
         <v>1041</v>
       </c>
@@ -17327,9 +17573,9 @@
       <c r="P162" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="R162" s="13"/>
-    </row>
-    <row r="163" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T162" s="13"/>
+    </row>
+    <row r="163" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="10" t="s">
         <v>1048</v>
       </c>
@@ -17361,11 +17607,11 @@
       <c r="Q163" s="13" t="s">
         <v>1051</v>
       </c>
-      <c r="R163" s="13" t="s">
+      <c r="T163" s="13" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="164" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
         <v>1053</v>
       </c>
@@ -17394,9 +17640,9 @@
       <c r="P164" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R164" s="13"/>
-    </row>
-    <row r="165" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T164" s="13"/>
+    </row>
+    <row r="165" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
         <v>1054</v>
       </c>
@@ -17425,9 +17671,9 @@
       <c r="P165" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R165" s="13"/>
-    </row>
-    <row r="166" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T165" s="13"/>
+    </row>
+    <row r="166" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="10" t="s">
         <v>1055</v>
       </c>
@@ -17460,9 +17706,9 @@
       <c r="P166" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R166" s="13"/>
-    </row>
-    <row r="167" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+      <c r="T166" s="13"/>
+    </row>
+    <row r="167" spans="1:20" ht="187" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
         <v>1059</v>
       </c>
@@ -17479,17 +17725,17 @@
         <v>1413</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>1750</v>
+        <v>1707</v>
       </c>
       <c r="G167" s="6" t="s">
-        <v>1694</v>
+        <v>1651</v>
       </c>
       <c r="H167" s="13" t="s">
         <v>230</v>
       </c>
       <c r="I167" s="13"/>
       <c r="L167" s="2" t="s">
-        <v>1778</v>
+        <v>1735</v>
       </c>
       <c r="N167" s="13"/>
       <c r="O167" s="13" t="s">
@@ -17498,14 +17744,20 @@
       <c r="P167" s="2" t="s">
         <v>1579</v>
       </c>
-      <c r="Q167" s="13" t="s">
-        <v>1646</v>
-      </c>
-      <c r="R167" s="13" t="s">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="Q167" s="2" t="s">
+        <v>1824</v>
+      </c>
+      <c r="R167" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="S167" s="13" t="s">
+        <v>1825</v>
+      </c>
+      <c r="T167" s="13" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A168" s="10" t="s">
         <v>1068</v>
       </c>
@@ -17520,7 +17772,7 @@
         <v>1413</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>1751</v>
+        <v>1708</v>
       </c>
       <c r="G168" s="12" t="s">
         <v>1427</v>
@@ -17531,24 +17783,30 @@
         <v>1413</v>
       </c>
       <c r="K168" s="14" t="s">
-        <v>1780</v>
+        <v>1737</v>
       </c>
       <c r="L168" s="2" t="s">
-        <v>1779</v>
+        <v>1736</v>
       </c>
       <c r="N168" s="13"/>
       <c r="O168" s="13"/>
       <c r="P168" s="2" t="s">
         <v>1580</v>
       </c>
-      <c r="Q168" s="13" t="s">
-        <v>1647</v>
-      </c>
-      <c r="R168" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q168" s="2" t="s">
+        <v>1827</v>
+      </c>
+      <c r="R168" s="2" t="s">
+        <v>1765</v>
+      </c>
+      <c r="S168" s="13" t="s">
+        <v>1826</v>
+      </c>
+      <c r="T168" s="13" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="10" t="s">
         <v>1074</v>
       </c>
@@ -17579,9 +17837,9 @@
       <c r="P169" s="2" t="s">
         <v>1075</v>
       </c>
-      <c r="R169" s="13"/>
-    </row>
-    <row r="170" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="T169" s="13"/>
+    </row>
+    <row r="170" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" s="10" t="s">
         <v>1076</v>
       </c>
@@ -17601,10 +17859,10 @@
         <v>1413</v>
       </c>
       <c r="K170" s="14" t="s">
-        <v>1782</v>
+        <v>1739</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>1781</v>
+        <v>1738</v>
       </c>
       <c r="N170" s="13"/>
       <c r="O170" s="13" t="s">
@@ -17613,14 +17871,14 @@
       <c r="P170" s="2" t="s">
         <v>1075</v>
       </c>
-      <c r="Q170" s="13" t="s">
-        <v>1648</v>
-      </c>
-      <c r="R170" s="13" t="s">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S170" s="13" t="s">
+        <v>1607</v>
+      </c>
+      <c r="T170" s="13" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="171" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="10" t="s">
         <v>1082</v>
       </c>
@@ -17649,9 +17907,9 @@
       <c r="P171" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R171" s="13"/>
-    </row>
-    <row r="172" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T171" s="13"/>
+    </row>
+    <row r="172" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="10" t="s">
         <v>1083</v>
       </c>
@@ -17680,9 +17938,9 @@
       <c r="P172" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R172" s="13"/>
-    </row>
-    <row r="173" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T172" s="13"/>
+    </row>
+    <row r="173" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="10" t="s">
         <v>1084</v>
       </c>
@@ -17711,9 +17969,9 @@
       <c r="P173" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R173" s="13"/>
-    </row>
-    <row r="174" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T173" s="13"/>
+    </row>
+    <row r="174" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A174" s="10" t="s">
         <v>1085</v>
       </c>
@@ -17726,7 +17984,7 @@
         <v>1413</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>1746</v>
+        <v>1703</v>
       </c>
       <c r="G174" s="12" t="s">
         <v>445</v>
@@ -17747,11 +18005,11 @@
         <v>1581</v>
       </c>
       <c r="Q174" s="13" t="s">
-        <v>1649</v>
-      </c>
-      <c r="R174" s="13"/>
-    </row>
-    <row r="175" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+        <v>1608</v>
+      </c>
+      <c r="T174" s="13"/>
+    </row>
+    <row r="175" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A175" s="10" t="s">
         <v>852</v>
       </c>
@@ -17764,7 +18022,7 @@
         <v>1413</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>1746</v>
+        <v>1703</v>
       </c>
       <c r="G175" s="12" t="s">
         <v>445</v>
@@ -17785,11 +18043,14 @@
         <v>1582</v>
       </c>
       <c r="Q175" s="13" t="s">
-        <v>1650</v>
-      </c>
-      <c r="R175" s="13"/>
-    </row>
-    <row r="176" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+        <v>1828</v>
+      </c>
+      <c r="R175" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="T175" s="13"/>
+    </row>
+    <row r="176" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" s="10" t="s">
         <v>1095</v>
       </c>
@@ -17802,10 +18063,10 @@
         <v>1413</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>1737</v>
+        <v>1694</v>
       </c>
       <c r="G176" s="12" t="s">
-        <v>1752</v>
+        <v>1709</v>
       </c>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
@@ -17822,14 +18083,14 @@
       <c r="P176" s="2" t="s">
         <v>1583</v>
       </c>
-      <c r="Q176" s="13" t="s">
+      <c r="S176" s="13" t="s">
         <v>611</v>
       </c>
-      <c r="R176" s="13" t="s">
+      <c r="T176" s="13" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="177" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="10" t="s">
         <v>1105</v>
       </c>
@@ -17861,9 +18122,9 @@
       <c r="P177" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R177" s="13"/>
-    </row>
-    <row r="178" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T177" s="13"/>
+    </row>
+    <row r="178" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="10" t="s">
         <v>1112</v>
       </c>
@@ -17896,11 +18157,11 @@
       <c r="P178" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R178" s="13" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T178" s="13" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>1120</v>
       </c>
@@ -17927,9 +18188,9 @@
       <c r="P179" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R179" s="13"/>
-    </row>
-    <row r="180" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="T179" s="13"/>
+    </row>
+    <row r="180" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
         <v>1121</v>
       </c>
@@ -17959,9 +18220,9 @@
       <c r="P180" s="2" t="s">
         <v>1584</v>
       </c>
-      <c r="R180" s="13"/>
-    </row>
-    <row r="181" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T180" s="13"/>
+    </row>
+    <row r="181" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
         <v>1136</v>
       </c>
@@ -17974,10 +18235,10 @@
         <v>1413</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>1754</v>
+        <v>1711</v>
       </c>
       <c r="G181" s="12" t="s">
-        <v>1753</v>
+        <v>1710</v>
       </c>
       <c r="H181" s="13"/>
       <c r="I181" s="14" t="s">
@@ -17993,9 +18254,9 @@
       <c r="P181" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R181" s="13"/>
-    </row>
-    <row r="182" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T181" s="13"/>
+    </row>
+    <row r="182" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
         <v>1140</v>
       </c>
@@ -18010,7 +18271,7 @@
         <v>1413</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>1755</v>
+        <v>1712</v>
       </c>
       <c r="G182" s="12" t="s">
         <v>1415</v>
@@ -18029,9 +18290,9 @@
       <c r="P182" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R182" s="13"/>
-    </row>
-    <row r="183" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="T182" s="13"/>
+    </row>
+    <row r="183" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
         <v>1151</v>
       </c>
@@ -18044,7 +18305,7 @@
         <v>2016</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>1756</v>
+        <v>1713</v>
       </c>
       <c r="G183" s="12" t="s">
         <v>1425</v>
@@ -18063,14 +18324,17 @@
       <c r="P183" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="Q183" s="13" t="s">
-        <v>1651</v>
-      </c>
-      <c r="R183" s="13" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q183" s="2" t="s">
+        <v>1829</v>
+      </c>
+      <c r="S183" s="13" t="s">
+        <v>1425</v>
+      </c>
+      <c r="T183" s="13" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="10" t="s">
         <v>1395</v>
       </c>
@@ -18081,9 +18345,9 @@
       <c r="P184" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R184" s="13"/>
-    </row>
-    <row r="185" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T184" s="13"/>
+    </row>
+    <row r="185" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="10" t="s">
         <v>1396</v>
       </c>
@@ -18098,9 +18362,9 @@
       <c r="P185" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R185" s="13"/>
-    </row>
-    <row r="186" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T185" s="13"/>
+    </row>
+    <row r="186" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="10" t="s">
         <v>1399</v>
       </c>
@@ -18113,9 +18377,9 @@
       <c r="P186" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R186" s="13"/>
-    </row>
-    <row r="187" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T186" s="13"/>
+    </row>
+    <row r="187" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="10" t="s">
         <v>1401</v>
       </c>
@@ -18126,9 +18390,9 @@
       <c r="P187" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R187" s="13"/>
-    </row>
-    <row r="188" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T187" s="13"/>
+    </row>
+    <row r="188" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="10" t="s">
         <v>1406</v>
       </c>
@@ -18139,9 +18403,9 @@
       <c r="P188" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R188" s="13"/>
-    </row>
-    <row r="189" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T188" s="13"/>
+    </row>
+    <row r="189" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="10" t="s">
         <v>974</v>
       </c>
@@ -18155,9 +18419,9 @@
       <c r="P189" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R189" s="13"/>
-    </row>
-    <row r="190" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T189" s="13"/>
+    </row>
+    <row r="190" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="10" t="s">
         <v>1153</v>
       </c>
@@ -18171,9 +18435,9 @@
       <c r="P190" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="R190" s="13"/>
-    </row>
-    <row r="191" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="T190" s="13"/>
+    </row>
+    <row r="191" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="10" t="s">
         <v>1409</v>
       </c>
@@ -18185,7 +18449,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="192" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="10" t="s">
         <v>1410</v>
       </c>
@@ -19195,7 +19459,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1757</v>
+        <v>1714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>